<commit_message>
Consensus Tree in checked
</commit_message>
<xml_diff>
--- a/data/finalist_dfs.xlsx
+++ b/data/finalist_dfs.xlsx
@@ -645,7 +645,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -745,7 +745,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
         <v>0.02455192732629511</v>
@@ -845,7 +845,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
         <v>0.006611278841703947</v>
@@ -945,7 +945,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
         <v>0.007362414872078041</v>
@@ -1145,7 +1145,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -1245,7 +1245,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -1445,7 +1445,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -1645,7 +1645,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -1845,7 +1845,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -1945,7 +1945,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -2045,7 +2045,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -2145,7 +2145,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
@@ -2345,7 +2345,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -2445,7 +2445,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
@@ -2545,7 +2545,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
@@ -2845,7 +2845,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
@@ -2945,7 +2945,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26" t="n">
         <v>0.04024839006439743</v>
@@ -3145,7 +3145,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
@@ -3245,7 +3245,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29" t="n">
         <v>0.1056462026059397</v>
@@ -3345,7 +3345,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
@@ -3445,7 +3445,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
@@ -3645,7 +3645,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C33" t="n">
         <v>0.009877518767285657</v>
@@ -3745,7 +3745,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
@@ -3945,7 +3945,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -4045,7 +4045,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C37" t="n">
         <v>0.006015218502812114</v>
@@ -4145,7 +4145,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38" t="n">
         <v>0.009785374127470806</v>
@@ -4245,7 +4245,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
@@ -4345,7 +4345,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
@@ -4445,7 +4445,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -4645,7 +4645,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
@@ -4745,7 +4745,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
@@ -4845,7 +4845,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
@@ -4945,7 +4945,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
@@ -5045,7 +5045,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
@@ -5145,7 +5145,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
@@ -5245,7 +5245,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
@@ -5345,7 +5345,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
@@ -5445,7 +5445,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
@@ -5545,7 +5545,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
@@ -5645,7 +5645,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C53" t="n">
         <v>0</v>
@@ -5745,7 +5745,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C54" t="n">
         <v>0</v>
@@ -5845,7 +5845,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C55" t="n">
         <v>0</v>
@@ -5945,7 +5945,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C56" t="n">
         <v>0</v>
@@ -6145,7 +6145,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C58" t="n">
         <v>0</v>
@@ -6345,7 +6345,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C60" t="n">
         <v>0.07006971937077391</v>
@@ -6445,7 +6445,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C61" t="n">
         <v>0</v>
@@ -6545,7 +6545,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C62" t="n">
         <v>0.1115656377835627</v>
@@ -6645,7 +6645,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C63" t="n">
         <v>0.01308329699084169</v>
@@ -6945,7 +6945,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C66" t="n">
         <v>0</v>
@@ -7045,7 +7045,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C67" t="n">
         <v>0</v>
@@ -7245,7 +7245,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C69" t="n">
         <v>0</v>
@@ -7742,7 +7742,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -7830,7 +7830,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -7918,7 +7918,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -8006,7 +8006,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -8094,7 +8094,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -8270,7 +8270,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -8534,7 +8534,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -8622,7 +8622,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="n">
         <v>0.3035</v>
@@ -8710,7 +8710,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -8974,7 +8974,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -9062,7 +9062,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
@@ -9326,7 +9326,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
@@ -9590,7 +9590,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" t="n">
         <v>3.5846</v>
@@ -9766,7 +9766,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
@@ -9854,7 +9854,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -9942,7 +9942,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
@@ -10030,7 +10030,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
@@ -10118,7 +10118,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
@@ -10206,7 +10206,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
@@ -10294,7 +10294,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
@@ -10382,7 +10382,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
@@ -10558,7 +10558,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C35" t="n">
         <v>2.0539</v>
@@ -10646,7 +10646,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -10822,7 +10822,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
@@ -10910,7 +10910,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
@@ -10998,7 +10998,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
@@ -11174,7 +11174,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
@@ -11262,7 +11262,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
@@ -11526,7 +11526,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C46" t="n">
         <v>3.7401</v>
@@ -11614,7 +11614,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
@@ -11702,7 +11702,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
@@ -11878,7 +11878,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
@@ -11966,7 +11966,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
@@ -12142,7 +12142,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C53" t="n">
         <v>0</v>
@@ -12230,7 +12230,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C54" t="n">
         <v>0.0154</v>
@@ -12494,7 +12494,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C57" t="n">
         <v>0</v>
@@ -12582,7 +12582,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C58" t="n">
         <v>0.0053</v>
@@ -12758,7 +12758,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C60" t="n">
         <v>0</v>
@@ -12934,7 +12934,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C62" t="n">
         <v>0</v>
@@ -13022,7 +13022,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C63" t="n">
         <v>0</v>
@@ -13198,7 +13198,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C65" t="n">
         <v>0</v>
@@ -13374,7 +13374,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C67" t="n">
         <v>0</v>
@@ -13638,7 +13638,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C70" t="n">
         <v>0</v>
@@ -13726,7 +13726,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C71" t="n">
         <v>0</v>

</xml_diff>